<commit_message>
modified schedule & update lin. algebra and MVN
</commit_message>
<xml_diff>
--- a/SCHEDULE.xlsx
+++ b/SCHEDULE.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25520" yWindow="720" windowWidth="25600" windowHeight="22960" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
   <si>
     <t>Week 1</t>
   </si>
@@ -126,12 +126,6 @@
     <t>Ch. 5 (Normal Model)</t>
   </si>
   <si>
-    <t>Ch. 7 (Multivariate Normal Model)</t>
-  </si>
-  <si>
-    <t>Ch. 6 (Gibbs Sampler &amp; multiple linear regression)</t>
-  </si>
-  <si>
     <t>Ch. 10 (Metropolis-Hastings algorithm)</t>
   </si>
   <si>
@@ -150,25 +144,25 @@
     <t>HW 3 posted</t>
   </si>
   <si>
-    <t>Ch. 9 (Linear Regression, will touch on Ch. 8 as special case, students must read both Ch. 8 and Ch. 9)</t>
-  </si>
-  <si>
     <t>HW 2 posted</t>
   </si>
   <si>
-    <t>NOTE: this schedule is only a template that I prepared before the course started.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">             As we make progress dates for important event may change. The most up-to date information will be provided in the class.</t>
-  </si>
-  <si>
-    <t>Poisson (application and influence of the prior)</t>
-  </si>
-  <si>
-    <t>MC Methods: compute predictive distribution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Approximate the posterior distribution of log(theta)</t>
+    <t>Ch. 6 (Gibbs Sampler)</t>
+  </si>
+  <si>
+    <t>Ch. 9 (Multiple Linear Regression)</t>
+  </si>
+  <si>
+    <t>Review of Linear Algebra &amp; MVN Dist.</t>
+  </si>
+  <si>
+    <t>Ch. 9 (Gibbs Sampler in the  linear regression).</t>
+  </si>
+  <si>
+    <t>Ch. 9 (Group comparisons &amp; Variable Selection)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tentative Schedule STT465, Fall, 2015.</t>
   </si>
 </sst>
 </file>
@@ -179,7 +173,7 @@
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -229,6 +223,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -375,7 +376,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="62">
+  <cellStyleXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -438,8 +439,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -500,8 +505,21 @@
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="62">
+  <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -532,6 +550,8 @@
     <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -563,6 +583,8 @@
     <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -895,520 +917,514 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:I34"/>
+  <dimension ref="B2:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection sqref="A1:G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
     <col min="4" max="4" width="10.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="33.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="45.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="35.83203125" customWidth="1"/>
+    <col min="7" max="7" width="3.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="20">
-      <c r="B1" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="2:9" ht="21" thickBot="1">
-      <c r="B2" s="28" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" ht="26" customHeight="1" thickBot="1">
-      <c r="B3" s="6" t="s">
+    <row r="2" spans="2:6" ht="23">
+      <c r="B2" s="36" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="21" thickBot="1">
+      <c r="B3" s="28"/>
+    </row>
+    <row r="4" spans="2:6" ht="26" customHeight="1" thickBot="1">
+      <c r="B4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="21" customHeight="1">
-      <c r="B4" s="10" t="s">
+    <row r="5" spans="2:6" ht="21" customHeight="1">
+      <c r="B5" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="12">
+      <c r="C5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="12">
         <v>42249</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E5" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F5" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="21" customHeight="1">
-      <c r="B5" s="14"/>
-      <c r="C5" s="2" t="s">
+    <row r="6" spans="2:6" ht="21" customHeight="1">
+      <c r="B6" s="14"/>
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="3">
-        <f>+D4+5</f>
+      <c r="D6" s="3">
+        <f>+D5+5</f>
         <v>42254</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="15" t="s">
+      <c r="E6" s="24"/>
+      <c r="F6" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="21" customHeight="1">
-      <c r="B6" s="14" t="s">
+    <row r="7" spans="2:6" ht="21" customHeight="1">
+      <c r="B7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="3">
-        <f>+D5+2</f>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3">
+        <f>+D6+2</f>
         <v>42256</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E7" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" ht="21" customHeight="1">
-      <c r="B7" s="17"/>
-      <c r="C7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="5">
-        <f>+D6+5</f>
-        <v>42261</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="18"/>
-    </row>
-    <row r="8" spans="2:9" ht="21" customHeight="1">
+      <c r="F7" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="21" customHeight="1">
       <c r="B8" s="17"/>
       <c r="C8" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D8" s="5">
-        <f>+D7+2</f>
+        <f>+D7+5</f>
+        <v>42261</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="18"/>
+    </row>
+    <row r="9" spans="2:6" ht="21" customHeight="1">
+      <c r="B9" s="17"/>
+      <c r="C9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="5">
+        <f>+D8+2</f>
         <v>42263</v>
       </c>
-      <c r="E8" s="30"/>
-      <c r="F8" s="18" t="s">
+      <c r="E9" s="33"/>
+      <c r="F9" s="18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="21" customHeight="1">
-      <c r="B9" s="14"/>
-      <c r="C9" s="2" t="s">
+    <row r="10" spans="2:6" ht="21" customHeight="1">
+      <c r="B10" s="14"/>
+      <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="3">
-        <f>+D8+5</f>
+      <c r="D10" s="3">
+        <f>+D9+5</f>
         <v>42268</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E10" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="16"/>
-    </row>
-    <row r="10" spans="2:9" ht="21" customHeight="1">
-      <c r="B10" s="14" t="s">
+      <c r="F10" s="16"/>
+    </row>
+    <row r="11" spans="2:6" ht="21" customHeight="1">
+      <c r="B11" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="3">
-        <f>+D9+2</f>
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3">
+        <f>+D10+2</f>
         <v>42270</v>
       </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="16" t="s">
+      <c r="E11" s="33"/>
+      <c r="F11" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="21" customHeight="1">
+      <c r="B12" s="17"/>
+      <c r="C12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="5">
+        <f>+D11+5</f>
+        <v>42275</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="18"/>
+    </row>
+    <row r="13" spans="2:6" ht="21" customHeight="1">
+      <c r="B13" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="5">
+        <f>+D12+2</f>
+        <v>42277</v>
+      </c>
+      <c r="E13" s="33"/>
+      <c r="F13" s="18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="21" customHeight="1">
+      <c r="B14" s="14"/>
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="3">
+        <f>+D13+5</f>
+        <v>42282</v>
+      </c>
+      <c r="E14" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="16"/>
+    </row>
+    <row r="15" spans="2:6" ht="21" customHeight="1">
+      <c r="B15" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="3">
+        <f>+D14+2</f>
+        <v>42284</v>
+      </c>
+      <c r="E15" s="33"/>
+      <c r="F15" s="16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="21" customHeight="1">
+      <c r="B16" s="17"/>
+      <c r="C16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="5">
+        <f>+D15+5</f>
+        <v>42289</v>
+      </c>
+      <c r="E16" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="H10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" ht="21" customHeight="1">
-      <c r="B11" s="17"/>
-      <c r="C11" s="4" t="s">
+      <c r="F16" s="18"/>
+    </row>
+    <row r="17" spans="2:6" ht="21" customHeight="1">
+      <c r="B17" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="5">
+        <f>+D16+2</f>
+        <v>42291</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="26" customHeight="1">
+      <c r="B18" s="14"/>
+      <c r="C18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="5">
-        <f>+D10+5</f>
-        <v>42275</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="18"/>
-      <c r="H11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" ht="21" customHeight="1">
-      <c r="B12" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="5">
-        <f>+D11+2</f>
-        <v>42277</v>
-      </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" ht="21" customHeight="1">
-      <c r="B13" s="14"/>
-      <c r="C13" s="2" t="s">
+      <c r="D18" s="3">
+        <f>+D17+5</f>
+        <v>42296</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="16"/>
+    </row>
+    <row r="19" spans="2:6" ht="21" customHeight="1">
+      <c r="B19" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="3">
+        <f>+D18+2</f>
+        <v>42298</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="16"/>
+    </row>
+    <row r="20" spans="2:6" ht="21" customHeight="1">
+      <c r="B20" s="17"/>
+      <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="3">
-        <f>+D12+5</f>
-        <v>42282</v>
-      </c>
-      <c r="E13" s="29" t="s">
+      <c r="D20" s="5">
+        <f>+D19+5</f>
+        <v>42303</v>
+      </c>
+      <c r="E20" s="26"/>
+      <c r="F20" s="18"/>
+    </row>
+    <row r="21" spans="2:6" ht="21" customHeight="1">
+      <c r="B21" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="5">
+        <f>+D20+2</f>
+        <v>42305</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="21" customHeight="1">
+      <c r="B22" s="14"/>
+      <c r="C22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="3">
+        <f>+D21+5</f>
+        <v>42310</v>
+      </c>
+      <c r="E22" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="16"/>
+    </row>
+    <row r="23" spans="2:6" ht="21" customHeight="1">
+      <c r="B23" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="3">
+        <f>+D22+2</f>
+        <v>42312</v>
+      </c>
+      <c r="E23" s="33"/>
+      <c r="F23" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="21" customHeight="1">
+      <c r="B24" s="17"/>
+      <c r="C24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="5">
+        <f>+D23+5</f>
+        <v>42317</v>
+      </c>
+      <c r="E24" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="16"/>
-    </row>
-    <row r="14" spans="2:9" ht="21" customHeight="1">
-      <c r="B14" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="3">
-        <f>+D13+2</f>
-        <v>42284</v>
-      </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" ht="21" customHeight="1">
-      <c r="B15" s="17"/>
-      <c r="C15" s="4" t="s">
+      <c r="F24" s="18"/>
+    </row>
+    <row r="25" spans="2:6" ht="21" customHeight="1">
+      <c r="B25" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="5">
+        <f>+D24+2</f>
+        <v>42319</v>
+      </c>
+      <c r="E25" s="33"/>
+      <c r="F25" s="18"/>
+    </row>
+    <row r="26" spans="2:6" ht="21" customHeight="1">
+      <c r="B26" s="14"/>
+      <c r="C26" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="5">
-        <f>+D14+5</f>
-        <v>42289</v>
-      </c>
-      <c r="E15" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" s="18"/>
-    </row>
-    <row r="16" spans="2:9" ht="21" customHeight="1">
-      <c r="B16" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="5">
-        <f>+D15+2</f>
-        <v>42291</v>
-      </c>
-      <c r="E16" s="30"/>
-      <c r="F16" s="18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="21" customHeight="1">
-      <c r="B17" s="14"/>
-      <c r="C17" s="2" t="s">
+      <c r="D26" s="3">
+        <f>+D25+5</f>
+        <v>42324</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" s="16"/>
+    </row>
+    <row r="27" spans="2:6" ht="21" customHeight="1">
+      <c r="B27" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="3">
+        <f>+D26+2</f>
+        <v>42326</v>
+      </c>
+      <c r="E27" s="33"/>
+      <c r="F27" s="16"/>
+    </row>
+    <row r="28" spans="2:6" ht="21" customHeight="1">
+      <c r="B28" s="17"/>
+      <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="3">
-        <f>+D16+5</f>
-        <v>42296</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" s="16"/>
-    </row>
-    <row r="18" spans="2:6" ht="21" customHeight="1">
-      <c r="B18" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="3">
-        <f>+D17+2</f>
-        <v>42298</v>
-      </c>
-      <c r="E18" s="30"/>
-      <c r="F18" s="16"/>
-    </row>
-    <row r="19" spans="2:6" ht="21" customHeight="1">
-      <c r="B19" s="17"/>
-      <c r="C19" s="4" t="s">
+      <c r="D28" s="5">
+        <f>+D27+5</f>
+        <v>42331</v>
+      </c>
+      <c r="E28" s="26"/>
+      <c r="F28" s="18"/>
+    </row>
+    <row r="29" spans="2:6" ht="21" customHeight="1">
+      <c r="B29" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="5">
+        <f>+D28+2</f>
+        <v>42333</v>
+      </c>
+      <c r="E29" s="26"/>
+      <c r="F29" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="21" customHeight="1">
+      <c r="B30" s="14"/>
+      <c r="C30" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="5">
-        <f>+D18+5</f>
-        <v>42303</v>
-      </c>
-      <c r="E19" s="26"/>
-      <c r="F19" s="18"/>
-    </row>
-    <row r="20" spans="2:6" ht="21" customHeight="1">
-      <c r="B20" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="5">
-        <f>+D19+2</f>
-        <v>42305</v>
-      </c>
-      <c r="E20" s="26"/>
-      <c r="F20" s="18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="21" customHeight="1">
-      <c r="B21" s="14"/>
-      <c r="C21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="3">
-        <f>+D20+5</f>
-        <v>42310</v>
-      </c>
-      <c r="E21" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="16"/>
-    </row>
-    <row r="22" spans="2:6" ht="21" customHeight="1">
-      <c r="B22" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="3">
-        <f>+D21+2</f>
-        <v>42312</v>
-      </c>
-      <c r="E22" s="30"/>
-      <c r="F22" s="16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" ht="21" customHeight="1">
-      <c r="B23" s="17"/>
-      <c r="C23" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="5">
-        <f>+D22+5</f>
-        <v>42317</v>
-      </c>
-      <c r="E23" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="F23" s="18"/>
-    </row>
-    <row r="24" spans="2:6" ht="21" customHeight="1">
-      <c r="B24" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="5">
-        <f>+D23+2</f>
-        <v>42319</v>
-      </c>
-      <c r="E24" s="30"/>
-      <c r="F24" s="18"/>
-    </row>
-    <row r="25" spans="2:6" ht="21" customHeight="1">
-      <c r="B25" s="14"/>
-      <c r="C25" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="3">
-        <f>+D24+5</f>
-        <v>42324</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="F25" s="16"/>
-    </row>
-    <row r="26" spans="2:6" ht="21" customHeight="1">
-      <c r="B26" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="3">
-        <f>+D25+2</f>
-        <v>42326</v>
-      </c>
-      <c r="E26" s="30"/>
-      <c r="F26" s="16"/>
-    </row>
-    <row r="27" spans="2:6" ht="21" customHeight="1">
-      <c r="B27" s="17"/>
-      <c r="C27" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="5">
-        <f>+D26+5</f>
-        <v>42331</v>
-      </c>
-      <c r="E27" s="26"/>
-      <c r="F27" s="18"/>
-    </row>
-    <row r="28" spans="2:6" ht="21" customHeight="1">
-      <c r="B28" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="5">
-        <f>+D27+2</f>
-        <v>42333</v>
-      </c>
-      <c r="E28" s="26"/>
-      <c r="F28" s="18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" ht="21" customHeight="1">
-      <c r="B29" s="14"/>
-      <c r="C29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="3">
-        <f>+D28+5</f>
+      <c r="D30" s="3">
+        <f>+D29+5</f>
         <v>42338</v>
-      </c>
-      <c r="E29" s="24"/>
-      <c r="F29" s="16"/>
-    </row>
-    <row r="30" spans="2:6" ht="21" customHeight="1">
-      <c r="B30" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="3">
-        <f>+D29+2</f>
-        <v>42340</v>
       </c>
       <c r="E30" s="24"/>
       <c r="F30" s="16"/>
     </row>
     <row r="31" spans="2:6" ht="21" customHeight="1">
-      <c r="B31" s="17"/>
-      <c r="C31" s="4" t="s">
+      <c r="B31" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="3">
+        <f>+D30+2</f>
+        <v>42340</v>
+      </c>
+      <c r="E31" s="24"/>
+      <c r="F31" s="16"/>
+    </row>
+    <row r="32" spans="2:6" ht="21" customHeight="1">
+      <c r="B32" s="17"/>
+      <c r="C32" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="5">
-        <f>+D30+5</f>
+      <c r="D32" s="5">
+        <f>+D31+5</f>
         <v>42345</v>
       </c>
-      <c r="E31" s="26"/>
-      <c r="F31" s="18"/>
-    </row>
-    <row r="32" spans="2:6" ht="21" customHeight="1">
-      <c r="B32" s="17" t="s">
+      <c r="E32" s="26"/>
+      <c r="F32" s="18"/>
+    </row>
+    <row r="33" spans="2:6" ht="21" customHeight="1">
+      <c r="B33" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="5">
-        <f>+D31+2</f>
+      <c r="C33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="5">
+        <f>+D32+2</f>
         <v>42347</v>
       </c>
-      <c r="E32" s="26"/>
-      <c r="F32" s="18" t="s">
+      <c r="E33" s="26"/>
+      <c r="F33" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="21" customHeight="1">
-      <c r="B33" s="14"/>
-      <c r="C33" s="2" t="s">
+    <row r="34" spans="2:6" ht="21" customHeight="1">
+      <c r="B34" s="14"/>
+      <c r="C34" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D33" s="3">
-        <f>+D32+5</f>
+      <c r="D34" s="3">
+        <f>+D33+5</f>
         <v>42352</v>
       </c>
-      <c r="E33" s="24"/>
-      <c r="F33" s="16" t="s">
+      <c r="E34" s="24"/>
+      <c r="F34" s="16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="2:6" ht="21" customHeight="1">
-      <c r="B34" s="19" t="s">
+    <row r="35" spans="2:6" ht="21" customHeight="1">
+      <c r="B35" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" s="21">
-        <f>+D33+2</f>
+      <c r="C35" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="21">
+        <f>+D34+2</f>
         <v>42354</v>
       </c>
-      <c r="E34" s="27"/>
-      <c r="F34" s="22"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="E17:E18"/>
+  <mergeCells count="7">
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="86" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="69" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>